<commit_message>
Updates after through question 7
</commit_message>
<xml_diff>
--- a/pa3/results.xlsx
+++ b/pa3/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bradwest/drive/msu/spring2019/csci566/csci566_pa/pa3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{722A1A70-FE08-0C40-96A5-4FB69E4E0094}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5AD981EF-314F-1A49-A331-E116FEC7F972}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="exp_1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="28">
   <si>
     <t>UDP</t>
   </si>
@@ -107,18 +107,43 @@
   <si>
     <t>*SQS is asynchronus, so there is no direct connection to the server and thus no connection time</t>
   </si>
+  <si>
+    <t>* Disallowed by SQS</t>
+  </si>
+  <si>
+    <t>*Not possible in SQS</t>
+  </si>
+  <si>
+    <t>*EC2 instance clocks are off :(</t>
+  </si>
+  <si>
+    <t>* No sqs messages dropped</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF555555"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -141,8 +166,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -896,15 +923,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -933,7 +960,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -952,8 +979,18 @@
       <c r="F2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G2">
+        <v>158.22268</v>
+      </c>
+      <c r="H2">
+        <v>2402.5729999999999</v>
+      </c>
+      <c r="I2">
+        <v>4545.7070000000003</v>
+      </c>
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -973,8 +1010,21 @@
         <f>F2*2</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G3">
+        <v>219.19155000000001</v>
+      </c>
+      <c r="H3">
+        <v>1790.7249999999999</v>
+      </c>
+      <c r="I3">
+        <v>3534.6509999999998</v>
+      </c>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -994,8 +1044,22 @@
         <f t="shared" ref="F4:F22" si="0">F3*2</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G4">
+        <v>82.851889999999997</v>
+      </c>
+      <c r="H4">
+        <v>1785.5160000000001</v>
+      </c>
+      <c r="I4">
+        <v>3544.6179999999999</v>
+      </c>
+      <c r="L4" s="2"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1015,8 +1079,22 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G5">
+        <v>47.29795</v>
+      </c>
+      <c r="H5">
+        <v>2008.951</v>
+      </c>
+      <c r="I5">
+        <v>4066.9389999999999</v>
+      </c>
+      <c r="L5" s="2"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -1036,8 +1114,22 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G6">
+        <v>50.00591</v>
+      </c>
+      <c r="H6">
+        <v>2536.9879999999998</v>
+      </c>
+      <c r="I6">
+        <v>4808.3549999999996</v>
+      </c>
+      <c r="L6" s="2"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -1057,8 +1149,22 @@
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G7">
+        <v>214.31136000000001</v>
+      </c>
+      <c r="H7">
+        <v>1876.174</v>
+      </c>
+      <c r="I7">
+        <v>3734.366</v>
+      </c>
+      <c r="L7" s="2"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1078,8 +1184,22 @@
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G8">
+        <v>79.519750000000002</v>
+      </c>
+      <c r="H8">
+        <v>1512.547</v>
+      </c>
+      <c r="I8">
+        <v>3227.17</v>
+      </c>
+      <c r="L8" s="2"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1099,8 +1219,22 @@
         <f t="shared" si="0"/>
         <v>128</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G9">
+        <v>47.55688</v>
+      </c>
+      <c r="H9">
+        <v>2329.7829999999999</v>
+      </c>
+      <c r="I9">
+        <v>3960.8339999999998</v>
+      </c>
+      <c r="L9" s="2"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -1120,8 +1254,22 @@
         <f t="shared" si="0"/>
         <v>256</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G10">
+        <v>38.237569999999998</v>
+      </c>
+      <c r="H10">
+        <v>2050.9839999999999</v>
+      </c>
+      <c r="I10">
+        <v>4118.1369999999997</v>
+      </c>
+      <c r="L10" s="2"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1141,8 +1289,22 @@
         <f t="shared" si="0"/>
         <v>512</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G11">
+        <v>53.53022</v>
+      </c>
+      <c r="H11">
+        <v>1779.231</v>
+      </c>
+      <c r="I11">
+        <v>3366.0459999999998</v>
+      </c>
+      <c r="L11" s="2"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1162,8 +1324,22 @@
         <f t="shared" si="0"/>
         <v>1024</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G12">
+        <v>62.758920000000003</v>
+      </c>
+      <c r="H12">
+        <v>1873.261</v>
+      </c>
+      <c r="I12">
+        <v>3790.3829999999998</v>
+      </c>
+      <c r="L12" s="2"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1183,8 +1359,22 @@
         <f t="shared" si="0"/>
         <v>2048</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G13">
+        <v>3338.12952</v>
+      </c>
+      <c r="H13">
+        <v>223878.408</v>
+      </c>
+      <c r="I13">
+        <v>480965.272</v>
+      </c>
+      <c r="L13" s="2"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -1204,8 +1394,22 @@
         <f t="shared" si="0"/>
         <v>4096</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G14">
+        <v>34637.191529999996</v>
+      </c>
+      <c r="H14">
+        <v>417348.995</v>
+      </c>
+      <c r="I14">
+        <v>806261.89599999995</v>
+      </c>
+      <c r="L14" s="2"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1225,8 +1429,22 @@
         <f t="shared" si="0"/>
         <v>8192</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G15">
+        <v>56777.378320000003</v>
+      </c>
+      <c r="H15">
+        <v>146595.69399999999</v>
+      </c>
+      <c r="I15">
+        <v>280524.03899999999</v>
+      </c>
+      <c r="L15" s="2"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1246,8 +1464,22 @@
         <f t="shared" si="0"/>
         <v>16384</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16">
+        <v>113.98887999999999</v>
+      </c>
+      <c r="H16">
+        <v>191411.788</v>
+      </c>
+      <c r="I16">
+        <v>455996.33600000001</v>
+      </c>
+      <c r="L16" s="2"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -1267,8 +1499,22 @@
         <f t="shared" si="0"/>
         <v>32768</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17">
+        <v>37859.207869999998</v>
+      </c>
+      <c r="H17">
+        <v>415620.16499999998</v>
+      </c>
+      <c r="I17">
+        <v>692237.54500000004</v>
+      </c>
+      <c r="L17" s="2"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1288,8 +1534,22 @@
         <f t="shared" si="0"/>
         <v>65536</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18">
+        <v>421.82540999999998</v>
+      </c>
+      <c r="H18">
+        <v>112541.63499999999</v>
+      </c>
+      <c r="I18">
+        <v>182906.883</v>
+      </c>
+      <c r="L18" s="2"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1309,8 +1569,22 @@
         <f t="shared" si="0"/>
         <v>131072</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19">
+        <v>518.32604000000003</v>
+      </c>
+      <c r="H19">
+        <v>3240.4780000000001</v>
+      </c>
+      <c r="I19">
+        <v>6343.1149999999998</v>
+      </c>
+      <c r="L19" s="2"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -1330,8 +1604,25 @@
         <f t="shared" si="0"/>
         <v>262144</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20" t="s">
+        <v>24</v>
+      </c>
+      <c r="L20" s="2"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -1351,8 +1642,17 @@
         <f t="shared" si="0"/>
         <v>524288</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1372,8 +1672,17 @@
         <f t="shared" si="0"/>
         <v>1048576</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1392,8 +1701,18 @@
       <c r="F23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G23">
+        <v>10.741</v>
+      </c>
+      <c r="H23">
+        <v>2336.5430000000001</v>
+      </c>
+      <c r="I23">
+        <v>4255.9660000000003</v>
+      </c>
+      <c r="M23" s="1"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1413,8 +1732,21 @@
         <f>F23*2</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G24">
+        <v>11.24287</v>
+      </c>
+      <c r="H24">
+        <v>1744.3969999999999</v>
+      </c>
+      <c r="I24">
+        <v>3505.16</v>
+      </c>
+      <c r="M24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -1434,8 +1766,22 @@
         <f t="shared" ref="F25:F43" si="1">F24*2</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G25">
+        <v>48.59066</v>
+      </c>
+      <c r="H25">
+        <v>1744.269</v>
+      </c>
+      <c r="I25">
+        <v>3390.6089999999999</v>
+      </c>
+      <c r="M25" s="2"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -1455,8 +1801,22 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G26">
+        <v>19.226310000000002</v>
+      </c>
+      <c r="H26">
+        <v>1941.0840000000001</v>
+      </c>
+      <c r="I26">
+        <v>3932.7730000000001</v>
+      </c>
+      <c r="M26" s="2"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -1476,8 +1836,22 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G27">
+        <v>15.546799999999999</v>
+      </c>
+      <c r="H27">
+        <v>2486.5169999999998</v>
+      </c>
+      <c r="I27">
+        <v>4782.1610000000001</v>
+      </c>
+      <c r="M27" s="2"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -1497,8 +1871,22 @@
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G28">
+        <v>11.382580000000001</v>
+      </c>
+      <c r="H28">
+        <v>1832.296</v>
+      </c>
+      <c r="I28">
+        <v>3710.6370000000002</v>
+      </c>
+      <c r="M28" s="2"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -1518,8 +1906,22 @@
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G29">
+        <v>19.107340000000001</v>
+      </c>
+      <c r="H29">
+        <v>1466.7329999999999</v>
+      </c>
+      <c r="I29">
+        <v>3085.0320000000002</v>
+      </c>
+      <c r="M29" s="2"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>22</v>
       </c>
@@ -1539,8 +1941,22 @@
         <f t="shared" si="1"/>
         <v>128</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G30">
+        <v>15.07258</v>
+      </c>
+      <c r="H30">
+        <v>2204.7139999999999</v>
+      </c>
+      <c r="I30">
+        <v>3751.19</v>
+      </c>
+      <c r="M30" s="2"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>22</v>
       </c>
@@ -1560,8 +1976,22 @@
         <f t="shared" si="1"/>
         <v>256</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G31">
+        <v>12.38608</v>
+      </c>
+      <c r="H31">
+        <v>1973.221</v>
+      </c>
+      <c r="I31">
+        <v>3825.4549999999999</v>
+      </c>
+      <c r="M31" s="2"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>22</v>
       </c>
@@ -1581,8 +2011,22 @@
         <f t="shared" si="1"/>
         <v>512</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G32">
+        <v>15.905379999999999</v>
+      </c>
+      <c r="H32">
+        <v>1725.6469999999999</v>
+      </c>
+      <c r="I32">
+        <v>3321.8510000000001</v>
+      </c>
+      <c r="M32" s="2"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>22</v>
       </c>
@@ -1602,8 +2046,22 @@
         <f t="shared" si="1"/>
         <v>1024</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G33">
+        <v>27.323720000000002</v>
+      </c>
+      <c r="H33">
+        <v>1810.634</v>
+      </c>
+      <c r="I33">
+        <v>3719.8359999999998</v>
+      </c>
+      <c r="M33" s="2"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>22</v>
       </c>
@@ -1623,8 +2081,22 @@
         <f t="shared" si="1"/>
         <v>2048</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G34">
+        <v>14.35852</v>
+      </c>
+      <c r="H34">
+        <v>330325.18199999997</v>
+      </c>
+      <c r="I34">
+        <v>485566.58100000001</v>
+      </c>
+      <c r="M34" s="2"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>22</v>
       </c>
@@ -1644,8 +2116,22 @@
         <f t="shared" si="1"/>
         <v>4096</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G35">
+        <v>14.107939999999999</v>
+      </c>
+      <c r="H35">
+        <v>527040.56499999994</v>
+      </c>
+      <c r="I35">
+        <v>808741.64300000004</v>
+      </c>
+      <c r="M35" s="2"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
+      <c r="Q35" s="1"/>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -1665,8 +2151,22 @@
         <f t="shared" si="1"/>
         <v>8192</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G36">
+        <v>12.64071</v>
+      </c>
+      <c r="H36">
+        <v>197786.21400000001</v>
+      </c>
+      <c r="I36">
+        <v>314788.50099999999</v>
+      </c>
+      <c r="M36" s="2"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="1"/>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>22</v>
       </c>
@@ -1686,8 +2186,22 @@
         <f t="shared" si="1"/>
         <v>16384</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G37">
+        <v>27.077909999999999</v>
+      </c>
+      <c r="H37">
+        <v>274050.57900000003</v>
+      </c>
+      <c r="I37">
+        <v>482826.77799999999</v>
+      </c>
+      <c r="M37" s="2"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1"/>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>22</v>
       </c>
@@ -1707,8 +2221,22 @@
         <f t="shared" si="1"/>
         <v>32768</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G38">
+        <v>45.4011</v>
+      </c>
+      <c r="H38">
+        <v>471477.33500000002</v>
+      </c>
+      <c r="I38">
+        <v>738512.95400000003</v>
+      </c>
+      <c r="M38" s="2"/>
+      <c r="N38" s="1"/>
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="1"/>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>22</v>
       </c>
@@ -1728,8 +2256,22 @@
         <f t="shared" si="1"/>
         <v>65536</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G39">
+        <v>84.708209999999994</v>
+      </c>
+      <c r="H39">
+        <v>122707.95</v>
+      </c>
+      <c r="I39">
+        <v>205957.31700000001</v>
+      </c>
+      <c r="M39" s="2"/>
+      <c r="N39" s="1"/>
+      <c r="O39" s="1"/>
+      <c r="P39" s="1"/>
+      <c r="Q39" s="1"/>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>22</v>
       </c>
@@ -1749,8 +2291,22 @@
         <f t="shared" si="1"/>
         <v>131072</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G40">
+        <v>183.84003999999999</v>
+      </c>
+      <c r="H40">
+        <v>2998.7950000000001</v>
+      </c>
+      <c r="I40">
+        <v>6071.9489999999996</v>
+      </c>
+      <c r="M40" s="2"/>
+      <c r="N40" s="1"/>
+      <c r="O40" s="1"/>
+      <c r="P40" s="1"/>
+      <c r="Q40" s="1"/>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>22</v>
       </c>
@@ -1770,8 +2326,25 @@
         <f t="shared" si="1"/>
         <v>262144</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41" t="s">
+        <v>24</v>
+      </c>
+      <c r="M41" s="2"/>
+      <c r="N41" s="1"/>
+      <c r="O41" s="1"/>
+      <c r="P41" s="1"/>
+      <c r="Q41" s="1"/>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>22</v>
       </c>
@@ -1791,8 +2364,17 @@
         <f t="shared" si="1"/>
         <v>524288</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>22</v>
       </c>
@@ -1811,6 +2393,194 @@
       <c r="F43">
         <f t="shared" si="1"/>
         <v>1048576</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:K5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2">
+        <v>30</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>32</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>30</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>32</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>30</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>32</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>30</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>32</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1818,12 +2588,1236 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:J5"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:S23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C5"/>
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>30</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>32</v>
+      </c>
+      <c r="G2">
+        <v>8.6829662322997994</v>
+      </c>
+      <c r="H2">
+        <v>1679.4831019181399</v>
+      </c>
+      <c r="I2">
+        <v>3470.0543880462601</v>
+      </c>
+      <c r="J2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" s="2"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>30</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <f>E2+0.2</f>
+        <v>0.2</v>
+      </c>
+      <c r="F3">
+        <v>32</v>
+      </c>
+      <c r="G3">
+        <v>-2.6273727416992099</v>
+      </c>
+      <c r="H3">
+        <v>1855.7672959107599</v>
+      </c>
+      <c r="I3">
+        <v>3677.0381927490198</v>
+      </c>
+      <c r="O3" s="2"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>30</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E12" si="0">E3+0.2</f>
+        <v>0.4</v>
+      </c>
+      <c r="F4">
+        <v>32</v>
+      </c>
+      <c r="G4">
+        <v>100.210666656494</v>
+      </c>
+      <c r="H4">
+        <v>1977.03566001011</v>
+      </c>
+      <c r="I4">
+        <v>3970.2131748199399</v>
+      </c>
+      <c r="O4" s="2"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>30</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="F5">
+        <v>32</v>
+      </c>
+      <c r="G5">
+        <v>-4.1818618774414</v>
+      </c>
+      <c r="H5">
+        <v>1614.25826182732</v>
+      </c>
+      <c r="I5">
+        <v>3343.14012527465</v>
+      </c>
+      <c r="O5" s="2"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>30</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+      <c r="F6">
+        <v>32</v>
+      </c>
+      <c r="G6">
+        <v>-1.58667564392089</v>
+      </c>
+      <c r="H6">
+        <v>1742.2083249458799</v>
+      </c>
+      <c r="I6">
+        <v>3486.8340492248499</v>
+      </c>
+      <c r="O6" s="2"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>30</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>32</v>
+      </c>
+      <c r="G7">
+        <v>-3.5901069641113201</v>
+      </c>
+      <c r="H7">
+        <v>1818.9711524889999</v>
+      </c>
+      <c r="I7">
+        <v>3586.52806282043</v>
+      </c>
+      <c r="O7" s="2"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>30</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="F8">
+        <v>32</v>
+      </c>
+      <c r="G8">
+        <v>-5.7439804077148402</v>
+      </c>
+      <c r="H8">
+        <v>2118.0795889634301</v>
+      </c>
+      <c r="I8">
+        <v>3787.3075008392302</v>
+      </c>
+      <c r="O8" s="2"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>30</v>
+      </c>
+      <c r="D9">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>1.4</v>
+      </c>
+      <c r="F9">
+        <v>32</v>
+      </c>
+      <c r="G9">
+        <v>-1.9562244415283201</v>
+      </c>
+      <c r="H9">
+        <v>2302.8056117204501</v>
+      </c>
+      <c r="I9">
+        <v>4449.7456550598099</v>
+      </c>
+      <c r="O9" s="2"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>30</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>1.5999999999999999</v>
+      </c>
+      <c r="F10">
+        <v>32</v>
+      </c>
+      <c r="G10">
+        <v>-4.22000885009765E-2</v>
+      </c>
+      <c r="H10">
+        <v>2201.3207123829702</v>
+      </c>
+      <c r="I10">
+        <v>4587.03589439392</v>
+      </c>
+      <c r="O10" s="2"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>30</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="F11">
+        <v>32</v>
+      </c>
+      <c r="G11">
+        <v>34.7540378570556</v>
+      </c>
+      <c r="H11">
+        <v>1948.3680037351701</v>
+      </c>
+      <c r="I11">
+        <v>3988.7452125549298</v>
+      </c>
+      <c r="O11" s="2"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>30</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>1.9999999999999998</v>
+      </c>
+      <c r="F12">
+        <v>32</v>
+      </c>
+      <c r="G12">
+        <v>4.0917396545410103</v>
+      </c>
+      <c r="H12">
+        <v>1533.6657808377099</v>
+      </c>
+      <c r="I12">
+        <v>3319.8380470275802</v>
+      </c>
+      <c r="N12" s="1"/>
+      <c r="S12" s="1"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>30</v>
+      </c>
+      <c r="D13">
+        <v>10</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>32</v>
+      </c>
+      <c r="G13">
+        <v>48.320293426513601</v>
+      </c>
+      <c r="H13">
+        <v>1728.4990273989099</v>
+      </c>
+      <c r="I13">
+        <v>3513.15355300903</v>
+      </c>
+      <c r="N13" s="2"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14">
+        <v>30</v>
+      </c>
+      <c r="D14">
+        <v>10</v>
+      </c>
+      <c r="E14">
+        <f>E13+0.2</f>
+        <v>0.2</v>
+      </c>
+      <c r="F14">
+        <v>32</v>
+      </c>
+      <c r="G14">
+        <v>65.473794937133704</v>
+      </c>
+      <c r="H14">
+        <v>1911.94980878096</v>
+      </c>
+      <c r="I14">
+        <v>3737.8602027892998</v>
+      </c>
+      <c r="N14" s="2"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15">
+        <v>30</v>
+      </c>
+      <c r="D15">
+        <v>10</v>
+      </c>
+      <c r="E15">
+        <f t="shared" ref="E15:E23" si="1">E14+0.2</f>
+        <v>0.4</v>
+      </c>
+      <c r="F15">
+        <v>32</v>
+      </c>
+      <c r="G15">
+        <v>147.34148979187</v>
+      </c>
+      <c r="H15">
+        <v>2034.3614862515301</v>
+      </c>
+      <c r="I15">
+        <v>4024.2800712585399</v>
+      </c>
+      <c r="N15" s="2"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16">
+        <v>30</v>
+      </c>
+      <c r="D16">
+        <v>10</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="F16">
+        <v>32</v>
+      </c>
+      <c r="G16">
+        <v>40.621757507324197</v>
+      </c>
+      <c r="H16">
+        <v>1750.0660923811099</v>
+      </c>
+      <c r="I16">
+        <v>3420.3085899353</v>
+      </c>
+      <c r="N16" s="2"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17">
+        <v>30</v>
+      </c>
+      <c r="D17">
+        <v>10</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>0.8</v>
+      </c>
+      <c r="F17">
+        <v>32</v>
+      </c>
+      <c r="G17">
+        <v>45.556068420410099</v>
+      </c>
+      <c r="H17">
+        <v>1800.2708279169501</v>
+      </c>
+      <c r="I17">
+        <v>3530.9283733367902</v>
+      </c>
+      <c r="N17" s="2"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18">
+        <v>30</v>
+      </c>
+      <c r="D18">
+        <v>10</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>32</v>
+      </c>
+      <c r="G18">
+        <v>137.29238510131799</v>
+      </c>
+      <c r="H18">
+        <v>1890.01496021564</v>
+      </c>
+      <c r="I18">
+        <v>3638.9615535736002</v>
+      </c>
+      <c r="N18" s="2"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19">
+        <v>30</v>
+      </c>
+      <c r="D19">
+        <v>10</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>1.2</v>
+      </c>
+      <c r="F19">
+        <v>32</v>
+      </c>
+      <c r="G19">
+        <v>39.891481399536097</v>
+      </c>
+      <c r="H19">
+        <v>2202.4409633416299</v>
+      </c>
+      <c r="I19">
+        <v>3934.0596199035599</v>
+      </c>
+      <c r="N19" s="2"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20">
+        <v>30</v>
+      </c>
+      <c r="D20">
+        <v>10</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>1.4</v>
+      </c>
+      <c r="F20">
+        <v>32</v>
+      </c>
+      <c r="G20">
+        <v>49.277782440185497</v>
+      </c>
+      <c r="H20">
+        <v>2362.2588882079399</v>
+      </c>
+      <c r="I20">
+        <v>4511.6307735443097</v>
+      </c>
+      <c r="N20" s="2"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21">
+        <v>30</v>
+      </c>
+      <c r="D21">
+        <v>10</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>1.5999999999999999</v>
+      </c>
+      <c r="F21">
+        <v>32</v>
+      </c>
+      <c r="G21">
+        <v>41.002273559570298</v>
+      </c>
+      <c r="H21">
+        <v>2289.7854034717202</v>
+      </c>
+      <c r="I21">
+        <v>4852.7500629425003</v>
+      </c>
+      <c r="N21" s="2"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22">
+        <v>30</v>
+      </c>
+      <c r="D22">
+        <v>10</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="1"/>
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="F22">
+        <v>32</v>
+      </c>
+      <c r="G22">
+        <v>75.609922409057603</v>
+      </c>
+      <c r="H22">
+        <v>2008.9215682102999</v>
+      </c>
+      <c r="I22">
+        <v>4030.5302143096901</v>
+      </c>
+      <c r="N22" s="2"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23">
+        <v>30</v>
+      </c>
+      <c r="D23">
+        <v>10</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>1.9999999999999998</v>
+      </c>
+      <c r="F23">
+        <v>32</v>
+      </c>
+      <c r="G23">
+        <v>51.130771636962798</v>
+      </c>
+      <c r="H23">
+        <v>1616.5976478503301</v>
+      </c>
+      <c r="I23">
+        <v>4442.5725936889603</v>
+      </c>
+      <c r="N23" s="2"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:K12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2">
+        <v>30</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>32</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>30</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E12" si="0">E2+0.2</f>
+        <v>0.2</v>
+      </c>
+      <c r="F3">
+        <v>32</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>30</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="F4">
+        <v>32</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>30</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="F5">
+        <v>32</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>30</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+      <c r="F6">
+        <v>32</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <v>30</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>32</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>30</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="F8">
+        <v>32</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9">
+        <v>30</v>
+      </c>
+      <c r="D9">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>1.4</v>
+      </c>
+      <c r="F9">
+        <v>32</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10">
+        <v>30</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>1.5999999999999999</v>
+      </c>
+      <c r="F10">
+        <v>32</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11">
+        <v>30</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="F11">
+        <v>32</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <v>30</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>1.9999999999999998</v>
+      </c>
+      <c r="F12">
+        <v>32</v>
+      </c>
+      <c r="G12">
+        <v>3</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:J23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1848,21 +3842,21 @@
         <v>16</v>
       </c>
       <c r="G1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="H1" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="I1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>30</v>
@@ -1877,131 +3871,22 @@
         <v>32</v>
       </c>
       <c r="G2">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3">
-        <v>30</v>
-      </c>
-      <c r="D3">
-        <v>10</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>32</v>
-      </c>
-      <c r="G3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4">
-        <v>30</v>
-      </c>
-      <c r="D4">
-        <v>10</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>32</v>
-      </c>
-      <c r="G4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5">
-        <v>30</v>
-      </c>
-      <c r="D5">
-        <v>10</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>32</v>
-      </c>
-      <c r="G5">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:I23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2">
-        <v>30</v>
-      </c>
-      <c r="D2">
-        <v>10</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
@@ -2018,8 +3903,20 @@
       <c r="F3">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
@@ -2036,8 +3933,20 @@
       <c r="F4">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -2054,8 +3963,20 @@
       <c r="F5">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -2072,8 +3993,20 @@
       <c r="F6">
         <v>32</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
@@ -2090,8 +4023,20 @@
       <c r="F7">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
@@ -2108,8 +4053,20 @@
       <c r="F8">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
@@ -2126,8 +4083,20 @@
       <c r="F9">
         <v>32</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
@@ -2144,8 +4113,20 @@
       <c r="F10">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
@@ -2162,8 +4143,20 @@
       <c r="F11">
         <v>32</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
       <c r="B12" t="s">
         <v>10</v>
       </c>
@@ -2180,8 +4173,20 @@
       <c r="F12">
         <v>32</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
@@ -2197,8 +4202,20 @@
       <c r="F13">
         <v>32</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
       <c r="B14" t="s">
         <v>11</v>
       </c>
@@ -2215,8 +4232,20 @@
       <c r="F14">
         <v>32</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
       <c r="B15" t="s">
         <v>11</v>
       </c>
@@ -2233,8 +4262,20 @@
       <c r="F15">
         <v>32</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
       <c r="B16" t="s">
         <v>11</v>
       </c>
@@ -2251,8 +4292,20 @@
       <c r="F16">
         <v>32</v>
       </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
       <c r="B17" t="s">
         <v>11</v>
       </c>
@@ -2269,8 +4322,20 @@
       <c r="F17">
         <v>32</v>
       </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
       <c r="B18" t="s">
         <v>11</v>
       </c>
@@ -2287,8 +4352,20 @@
       <c r="F18">
         <v>32</v>
       </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
       <c r="B19" t="s">
         <v>11</v>
       </c>
@@ -2305,8 +4382,20 @@
       <c r="F19">
         <v>32</v>
       </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
       <c r="B20" t="s">
         <v>11</v>
       </c>
@@ -2323,8 +4412,20 @@
       <c r="F20">
         <v>32</v>
       </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
       <c r="B21" t="s">
         <v>11</v>
       </c>
@@ -2341,8 +4442,20 @@
       <c r="F21">
         <v>32</v>
       </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
       <c r="B22" t="s">
         <v>11</v>
       </c>
@@ -2359,8 +4472,20 @@
       <c r="F22">
         <v>32</v>
       </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
       <c r="B23" t="s">
         <v>11</v>
       </c>
@@ -2377,720 +4502,14 @@
       <c r="F23">
         <v>32</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:J12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2">
-        <v>30</v>
-      </c>
-      <c r="D2">
-        <v>10</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>32</v>
-      </c>
-      <c r="G2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3">
-        <v>30</v>
-      </c>
-      <c r="D3">
-        <v>10</v>
-      </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E12" si="0">E2+0.2</f>
-        <v>0.2</v>
-      </c>
-      <c r="F3">
-        <v>32</v>
-      </c>
-      <c r="G3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4">
-        <v>30</v>
-      </c>
-      <c r="D4">
-        <v>10</v>
-      </c>
-      <c r="E4">
-        <f t="shared" si="0"/>
-        <v>0.4</v>
-      </c>
-      <c r="F4">
-        <v>32</v>
-      </c>
-      <c r="G4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5">
-        <v>30</v>
-      </c>
-      <c r="D5">
-        <v>10</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="0"/>
-        <v>0.60000000000000009</v>
-      </c>
-      <c r="F5">
-        <v>32</v>
-      </c>
-      <c r="G5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6">
-        <v>30</v>
-      </c>
-      <c r="D6">
-        <v>10</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="0"/>
-        <v>0.8</v>
-      </c>
-      <c r="F6">
-        <v>32</v>
-      </c>
-      <c r="G6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7">
-        <v>30</v>
-      </c>
-      <c r="D7">
-        <v>10</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>32</v>
-      </c>
-      <c r="G7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8">
-        <v>30</v>
-      </c>
-      <c r="D8">
-        <v>10</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="0"/>
-        <v>1.2</v>
-      </c>
-      <c r="F8">
-        <v>32</v>
-      </c>
-      <c r="G8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9">
-        <v>30</v>
-      </c>
-      <c r="D9">
-        <v>10</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="0"/>
-        <v>1.4</v>
-      </c>
-      <c r="F9">
-        <v>32</v>
-      </c>
-      <c r="G9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10">
-        <v>30</v>
-      </c>
-      <c r="D10">
-        <v>10</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="0"/>
-        <v>1.5999999999999999</v>
-      </c>
-      <c r="F10">
-        <v>32</v>
-      </c>
-      <c r="G10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11">
-        <v>30</v>
-      </c>
-      <c r="D11">
-        <v>10</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="0"/>
-        <v>1.7999999999999998</v>
-      </c>
-      <c r="F11">
-        <v>32</v>
-      </c>
-      <c r="G11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12">
-        <v>30</v>
-      </c>
-      <c r="D12">
-        <v>10</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="0"/>
-        <v>1.9999999999999998</v>
-      </c>
-      <c r="F12">
-        <v>32</v>
-      </c>
-      <c r="G12">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:I23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2">
-        <v>30</v>
-      </c>
-      <c r="D2">
-        <v>10</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3">
-        <v>30</v>
-      </c>
-      <c r="D3">
-        <v>10</v>
-      </c>
-      <c r="E3">
-        <f>E2+0.2</f>
-        <v>0.2</v>
-      </c>
-      <c r="F3">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4">
-        <v>30</v>
-      </c>
-      <c r="D4">
-        <v>10</v>
-      </c>
-      <c r="E4">
-        <f t="shared" ref="E4:E12" si="0">E3+0.2</f>
-        <v>0.4</v>
-      </c>
-      <c r="F4">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5">
-        <v>30</v>
-      </c>
-      <c r="D5">
-        <v>10</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="0"/>
-        <v>0.60000000000000009</v>
-      </c>
-      <c r="F5">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6">
-        <v>30</v>
-      </c>
-      <c r="D6">
-        <v>10</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="0"/>
-        <v>0.8</v>
-      </c>
-      <c r="F6">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7">
-        <v>30</v>
-      </c>
-      <c r="D7">
-        <v>10</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8">
-        <v>30</v>
-      </c>
-      <c r="D8">
-        <v>10</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="0"/>
-        <v>1.2</v>
-      </c>
-      <c r="F8">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9">
-        <v>30</v>
-      </c>
-      <c r="D9">
-        <v>10</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="0"/>
-        <v>1.4</v>
-      </c>
-      <c r="F9">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10">
-        <v>30</v>
-      </c>
-      <c r="D10">
-        <v>10</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="0"/>
-        <v>1.5999999999999999</v>
-      </c>
-      <c r="F10">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11">
-        <v>30</v>
-      </c>
-      <c r="D11">
-        <v>10</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="0"/>
-        <v>1.7999999999999998</v>
-      </c>
-      <c r="F11">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12">
-        <v>30</v>
-      </c>
-      <c r="D12">
-        <v>10</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="0"/>
-        <v>1.9999999999999998</v>
-      </c>
-      <c r="F12">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13">
-        <v>30</v>
-      </c>
-      <c r="D13">
-        <v>10</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14">
-        <v>30</v>
-      </c>
-      <c r="D14">
-        <v>10</v>
-      </c>
-      <c r="E14">
-        <f>E13+0.2</f>
-        <v>0.2</v>
-      </c>
-      <c r="F14">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15">
-        <v>30</v>
-      </c>
-      <c r="D15">
-        <v>10</v>
-      </c>
-      <c r="E15">
-        <f t="shared" ref="E15:E23" si="1">E14+0.2</f>
-        <v>0.4</v>
-      </c>
-      <c r="F15">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16">
-        <v>30</v>
-      </c>
-      <c r="D16">
-        <v>10</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="1"/>
-        <v>0.60000000000000009</v>
-      </c>
-      <c r="F16">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17">
-        <v>30</v>
-      </c>
-      <c r="D17">
-        <v>10</v>
-      </c>
-      <c r="E17">
-        <f t="shared" si="1"/>
-        <v>0.8</v>
-      </c>
-      <c r="F17">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18">
-        <v>30</v>
-      </c>
-      <c r="D18">
-        <v>10</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F18">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19">
-        <v>30</v>
-      </c>
-      <c r="D19">
-        <v>10</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="1"/>
-        <v>1.2</v>
-      </c>
-      <c r="F19">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20">
-        <v>30</v>
-      </c>
-      <c r="D20">
-        <v>10</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="1"/>
-        <v>1.4</v>
-      </c>
-      <c r="F20">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B21" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21">
-        <v>30</v>
-      </c>
-      <c r="D21">
-        <v>10</v>
-      </c>
-      <c r="E21">
-        <f t="shared" si="1"/>
-        <v>1.5999999999999999</v>
-      </c>
-      <c r="F21">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22">
-        <v>30</v>
-      </c>
-      <c r="D22">
-        <v>10</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="1"/>
-        <v>1.7999999999999998</v>
-      </c>
-      <c r="F22">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23">
-        <v>30</v>
-      </c>
-      <c r="D23">
-        <v>10</v>
-      </c>
-      <c r="E23">
-        <f t="shared" si="1"/>
-        <v>1.9999999999999998</v>
-      </c>
-      <c r="F23">
-        <v>32</v>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3100,15 +4519,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C12"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -3140,7 +4559,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>12</v>
       </c>
@@ -3159,8 +4578,20 @@
       <c r="G2">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -3180,8 +4611,17 @@
       <c r="G3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>12</v>
       </c>
@@ -3201,8 +4641,17 @@
       <c r="G4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>12</v>
       </c>
@@ -3222,8 +4671,17 @@
       <c r="G5">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>12</v>
       </c>
@@ -3243,8 +4701,17 @@
       <c r="G6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>12</v>
       </c>
@@ -3264,8 +4731,17 @@
       <c r="G7">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>12</v>
       </c>
@@ -3285,8 +4761,17 @@
       <c r="G8">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>12</v>
       </c>
@@ -3306,8 +4791,17 @@
       <c r="G9">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>12</v>
       </c>
@@ -3327,8 +4821,17 @@
       <c r="G10">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>12</v>
       </c>
@@ -3348,8 +4851,17 @@
       <c r="G11">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>12</v>
       </c>
@@ -3368,6 +4880,15 @@
       </c>
       <c r="G12">
         <v>3</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add question 10 results and code
</commit_message>
<xml_diff>
--- a/pa3/results.xlsx
+++ b/pa3/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bradwest/drive/msu/spring2019/csci566/csci566_pa/pa3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5AD981EF-314F-1A49-A331-E116FEC7F972}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4B520304-512B-7547-88CD-77850B3DC972}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="exp_1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="28">
   <si>
     <t>UDP</t>
   </si>
@@ -540,15 +540,15 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -580,7 +580,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -599,8 +602,21 @@
       <c r="G2">
         <v>256</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H2">
+        <v>47.416210174560497</v>
+      </c>
+      <c r="I2">
+        <v>1840.4499567472001</v>
+      </c>
+      <c r="J2">
+        <v>3599.7326374053901</v>
+      </c>
+      <c r="N2" s="1"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
@@ -620,8 +636,25 @@
         <f>G2/2</f>
         <v>128</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H3">
+        <v>2655.94387054443</v>
+      </c>
+      <c r="I3">
+        <v>4463.19315525201</v>
+      </c>
+      <c r="J3">
+        <v>6259.5577239990198</v>
+      </c>
+      <c r="N3" s="2"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
@@ -641,8 +674,25 @@
         <f t="shared" ref="G4:G10" si="0">G3/2</f>
         <v>64</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H4">
+        <v>5830.8584690093903</v>
+      </c>
+      <c r="I4">
+        <v>7679.0393453377901</v>
+      </c>
+      <c r="J4">
+        <v>9359.6909046173005</v>
+      </c>
+      <c r="N4" s="2"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
@@ -662,8 +712,25 @@
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H5">
+        <v>9344.7067737579291</v>
+      </c>
+      <c r="I5">
+        <v>11072.231920865799</v>
+      </c>
+      <c r="J5">
+        <v>12817.7707195281</v>
+      </c>
+      <c r="N5" s="2"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
@@ -683,8 +750,25 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H6">
+        <v>12758.285999297999</v>
+      </c>
+      <c r="I6">
+        <v>14580.3457681949</v>
+      </c>
+      <c r="J6">
+        <v>16452.364683151201</v>
+      </c>
+      <c r="N6" s="2"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
@@ -704,8 +788,25 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H7">
+        <v>16401.504755020102</v>
+      </c>
+      <c r="I7">
+        <v>18241.6293391814</v>
+      </c>
+      <c r="J7">
+        <v>20045.968770980799</v>
+      </c>
+      <c r="N7" s="2"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
@@ -725,8 +826,25 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H8">
+        <v>20047.175407409599</v>
+      </c>
+      <c r="I8">
+        <v>21819.731088785</v>
+      </c>
+      <c r="J8">
+        <v>23524.977684020902</v>
+      </c>
+      <c r="N8" s="2"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
@@ -746,8 +864,25 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H9">
+        <v>23581.831693649201</v>
+      </c>
+      <c r="I9">
+        <v>25369.312286376899</v>
+      </c>
+      <c r="J9">
+        <v>27310.919046401901</v>
+      </c>
+      <c r="N9" s="2"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
@@ -767,6 +902,27 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="H10">
+        <v>27339.115381240801</v>
+      </c>
+      <c r="I10">
+        <v>28957.0198013232</v>
+      </c>
+      <c r="J10">
+        <v>30896.021604537898</v>
+      </c>
+      <c r="N10" s="2"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="N11" s="2"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3816,7 +3972,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
@@ -4522,7 +4678,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4560,6 +4716,9 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
       <c r="B2" t="s">
         <v>12</v>
       </c>
@@ -4592,6 +4751,9 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -4622,6 +4784,9 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
       <c r="B4" t="s">
         <v>12</v>
       </c>
@@ -4652,6 +4817,9 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
       <c r="B5" t="s">
         <v>12</v>
       </c>
@@ -4682,6 +4850,9 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
       <c r="B6" t="s">
         <v>12</v>
       </c>
@@ -4712,6 +4883,9 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
@@ -4742,6 +4916,9 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
@@ -4772,6 +4949,9 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
       <c r="B9" t="s">
         <v>12</v>
       </c>
@@ -4802,6 +4982,9 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
       <c r="B10" t="s">
         <v>12</v>
       </c>
@@ -4832,6 +5015,9 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
       <c r="B11" t="s">
         <v>12</v>
       </c>
@@ -4862,6 +5048,9 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
       <c r="B12" t="s">
         <v>12</v>
       </c>
@@ -4901,7 +5090,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C22"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4930,6 +5119,9 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
@@ -4947,6 +5139,9 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
@@ -4965,6 +5160,9 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
@@ -4983,6 +5181,9 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -5001,6 +5202,9 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -5019,6 +5223,9 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
@@ -5037,6 +5244,9 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
@@ -5055,6 +5265,9 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
@@ -5073,6 +5286,9 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
@@ -5091,6 +5307,9 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
@@ -5109,6 +5328,9 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
       <c r="B12" t="s">
         <v>10</v>
       </c>
@@ -5127,6 +5349,9 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
       <c r="B13" t="s">
         <v>10</v>
       </c>
@@ -5145,6 +5370,9 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
       <c r="B14" t="s">
         <v>10</v>
       </c>
@@ -5163,6 +5391,9 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
       <c r="B15" t="s">
         <v>10</v>
       </c>
@@ -5181,6 +5412,9 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
       <c r="B16" t="s">
         <v>10</v>
       </c>
@@ -5198,7 +5432,10 @@
         <v>16384</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
       <c r="B17" t="s">
         <v>10</v>
       </c>
@@ -5216,7 +5453,10 @@
         <v>32768</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
       <c r="B18" t="s">
         <v>10</v>
       </c>
@@ -5234,7 +5474,10 @@
         <v>65536</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
       <c r="B19" t="s">
         <v>10</v>
       </c>
@@ -5252,7 +5495,10 @@
         <v>131072</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
       <c r="B20" t="s">
         <v>10</v>
       </c>
@@ -5270,7 +5516,10 @@
         <v>262144</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
       <c r="B21" t="s">
         <v>10</v>
       </c>
@@ -5288,7 +5537,10 @@
         <v>524288</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
       <c r="B22" t="s">
         <v>10</v>
       </c>

</xml_diff>